<commit_message>
add ver1 (for reference)
</commit_message>
<xml_diff>
--- a/data-scientist-skill-checklist-ver2-20171025.xlsx
+++ b/data-scientist-skill-checklist-ver2-20171025.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>NO</t>
   </si>
@@ -127,6 +127,10 @@
   <si>
     <t>データを取り扱う⼈間として相応しい倫理を⾝に着けている（データのねつ造、改
 ざん、盗⽤を⾏わないなど）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> B-0003. 作業ありきではなく、本質的な問題（イシュー）ありきで行動できる</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -466,7 +470,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -651,7 +655,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="27" x14ac:dyDescent="0.15">
       <c r="B8" s="2">
         <v>7</v>
       </c>
@@ -660,6 +664,9 @@
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>